<commit_message>
Made changes as per discussed in the final version of the website
</commit_message>
<xml_diff>
--- a/data/subs_table.xlsx
+++ b/data/subs_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\artranslation\artranslator\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huzefasadikot/Desktop/Kiki_Website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1908A113-030D-40B3-A228-B3CE40A26C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA34518-C064-AE4B-BB71-A5BAE4ADDBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,12 +75,6 @@
     <t>Purrfect Pals (Free)</t>
   </si>
   <si>
-    <t>Whisker Whispers ($2)</t>
-  </si>
-  <si>
-    <t>Meow Majesty ($5)</t>
-  </si>
-  <si>
     <t>AI-Chat on your Server with Image Vision capabilities</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>Select between Simple or Advanced translation themes</t>
   </si>
   <si>
-    <t>Feline Finest ($10)</t>
-  </si>
-  <si>
     <t>/set_1_lang</t>
   </si>
   <si>
@@ -163,6 +154,15 @@
   </si>
   <si>
     <t>React with Loudspeaker 📢 emoji</t>
+  </si>
+  <si>
+    <t>Whisker Whispers (1 Token)</t>
+  </si>
+  <si>
+    <t>Meow Majesty (2 Tokens)</t>
+  </si>
+  <si>
+    <t>Feline Finest (5 Tokens)</t>
   </si>
 </sst>
 </file>
@@ -488,21 +488,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="68.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
@@ -510,32 +510,32 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -550,12 +550,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -570,33 +570,33 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
@@ -610,13 +610,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
@@ -630,12 +630,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
@@ -650,12 +650,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
@@ -670,12 +670,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
@@ -690,12 +690,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>14</v>
@@ -710,12 +710,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
@@ -730,12 +730,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
@@ -750,12 +750,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
@@ -770,12 +770,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>14</v>
@@ -790,12 +790,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
@@ -810,12 +810,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>14</v>
@@ -830,12 +830,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>14</v>
@@ -850,12 +850,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>14</v>
@@ -870,12 +870,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>14</v>
@@ -890,7 +890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25"/>
     </row>
   </sheetData>

</xml_diff>